<commit_message>
Logboek bijgewerkt sheet Ruud
</commit_message>
<xml_diff>
--- a/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
+++ b/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wander" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>vb: 19/04/2016</t>
+  </si>
+  <si>
+    <t>Woensdag</t>
+  </si>
+  <si>
+    <t>Introductie</t>
+  </si>
+  <si>
+    <t>Maandag</t>
+  </si>
+  <si>
+    <t>Opdracht bedenken en omschrijven</t>
+  </si>
+  <si>
+    <t>Gesprek Opdrachtgever en Tutor + Userstories aangemaakt + Logboek gemaakt + Github repository gestart + Trello</t>
   </si>
 </sst>
 </file>
@@ -209,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -237,6 +252,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,7 +2067,7 @@
   <dimension ref="A5:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2648,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,33 +2721,69 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="11">
+        <v>42473</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="11">
+        <v>42478</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>42479</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8">
+        <v>16</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="11">
+        <v>42114</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8">
+        <v>16</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>

</xml_diff>

<commit_message>
LOgboek update sheet RUud
</commit_message>
<xml_diff>
--- a/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
+++ b/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ruud\Gedeelde bestanden\P4P-chatbot\Logboek\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19290" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wander" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -116,11 +121,20 @@
   <si>
     <t>Donderdag</t>
   </si>
+  <si>
+    <t>Introductie</t>
+  </si>
+  <si>
+    <t>Opdracht bedenken en omschrijven</t>
+  </si>
+  <si>
+    <t>Gesprek Opdrachtgever en Tutor + Userstories aangemaakt + Logboek gemaakt + Github repository gestart + Trello</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,7 +904,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -901,13 +918,13 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,7 +948,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -951,7 +968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -959,7 +976,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -967,7 +984,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -975,7 +992,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -983,7 +1000,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -991,7 +1008,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -999,7 +1016,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1007,7 +1024,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1015,7 +1032,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1023,7 +1040,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1031,7 +1048,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1039,7 +1056,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1047,7 +1064,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1055,7 +1072,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1063,7 +1080,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1071,7 +1088,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1079,7 +1096,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1087,7 +1104,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1095,7 +1112,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1103,7 +1120,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1111,7 +1128,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1119,7 +1136,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1127,7 +1144,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1135,7 +1152,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1143,7 +1160,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1151,7 +1168,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1159,7 +1176,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1167,7 +1184,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1175,7 +1192,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1183,7 +1200,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1191,7 +1208,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1199,7 +1216,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1207,7 +1224,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1215,7 +1232,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1223,7 +1240,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1231,7 +1248,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1239,7 +1256,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1247,7 +1264,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1255,7 +1272,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1263,7 +1280,7 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1271,7 +1288,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1279,7 +1296,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1287,7 +1304,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1295,7 +1312,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1303,7 +1320,7 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1311,7 +1328,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1319,7 +1336,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1327,7 +1344,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1335,7 +1352,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1343,7 +1360,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1351,7 +1368,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1359,7 +1376,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1367,7 +1384,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1375,7 +1392,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1383,7 +1400,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1391,7 +1408,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1399,7 +1416,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1407,7 +1424,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1415,7 +1432,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1423,7 +1440,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1431,7 +1448,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1439,7 +1456,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1447,7 +1464,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1455,7 +1472,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1463,7 +1480,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1471,7 +1488,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1479,7 +1496,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1502,13 +1519,13 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1532,7 +1549,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -1552,7 +1569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1560,7 +1577,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1568,7 +1585,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1576,7 +1593,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1584,7 +1601,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1592,7 +1609,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1600,7 +1617,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1608,7 +1625,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1616,7 +1633,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1624,7 +1641,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1632,7 +1649,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1640,7 +1657,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1648,7 +1665,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1656,7 +1673,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1664,7 +1681,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1672,7 +1689,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1680,7 +1697,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1688,7 +1705,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1696,7 +1713,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1704,7 +1721,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1712,7 +1729,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1720,7 +1737,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1728,7 +1745,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1736,7 +1753,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1744,7 +1761,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1752,7 +1769,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1760,7 +1777,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1768,7 +1785,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1776,7 +1793,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1784,7 +1801,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1792,7 +1809,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1800,7 +1817,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1808,7 +1825,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1816,7 +1833,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1824,7 +1841,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1832,7 +1849,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1840,7 +1857,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1848,7 +1865,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1856,7 +1873,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1864,7 +1881,7 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1872,7 +1889,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1880,7 +1897,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1888,7 +1905,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1896,7 +1913,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1904,7 +1921,7 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1912,7 +1929,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1920,7 +1937,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1928,7 +1945,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1936,7 +1953,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1944,7 +1961,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1952,7 +1969,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1960,7 +1977,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1968,7 +1985,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1976,7 +1993,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1984,7 +2001,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1992,7 +2009,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2000,7 +2017,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -2008,7 +2025,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2016,7 +2033,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -2024,7 +2041,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2032,7 +2049,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -2040,7 +2057,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2048,7 +2065,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2056,7 +2073,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2064,7 +2081,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2072,7 +2089,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2080,7 +2097,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2098,17 +2115,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2132,7 +2149,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2150,7 +2167,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
@@ -2170,7 +2187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
@@ -2188,7 +2205,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
@@ -2206,7 +2223,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>21</v>
       </c>
@@ -2220,7 +2237,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -2228,7 +2245,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -2236,7 +2253,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -2244,7 +2261,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -2252,7 +2269,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -2260,7 +2277,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -2268,7 +2285,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -2276,7 +2293,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -2284,7 +2301,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -2292,7 +2309,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -2300,7 +2317,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -2308,7 +2325,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2316,7 +2333,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -2324,7 +2341,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -2332,7 +2349,7 @@
       <c r="E24" s="13"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -2340,7 +2357,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -2348,7 +2365,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -2356,7 +2373,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -2364,7 +2381,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -2372,7 +2389,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -2380,7 +2397,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2388,7 +2405,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2396,7 +2413,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2404,7 +2421,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2412,7 +2429,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2420,7 +2437,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2428,7 +2445,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2436,7 +2453,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2444,7 +2461,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2452,7 +2469,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2460,7 +2477,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2468,7 +2485,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2476,7 +2493,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2484,7 +2501,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2492,7 +2509,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2500,7 +2517,7 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2508,7 +2525,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -2516,7 +2533,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -2524,7 +2541,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2532,7 +2549,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2540,7 +2557,7 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2548,7 +2565,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2556,7 +2573,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2564,7 +2581,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2572,7 +2589,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2580,7 +2597,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2588,7 +2605,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2596,7 +2613,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2604,7 +2621,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2612,7 +2629,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2620,7 +2637,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2628,7 +2645,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2636,7 +2653,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -2644,7 +2661,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2652,7 +2669,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -2660,7 +2677,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2668,7 +2685,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -2676,7 +2693,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2684,7 +2701,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2692,7 +2709,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2700,7 +2717,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2708,7 +2725,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2716,7 +2733,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2735,17 +2752,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2769,7 +2786,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2789,39 +2806,75 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>42473</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>42478</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="8">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>42479</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8">
+        <v>16</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>42114</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8">
+        <v>16</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2829,7 +2882,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2837,7 +2890,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2845,7 +2898,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2853,7 +2906,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2861,7 +2914,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2869,7 +2922,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2877,7 +2930,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2885,7 +2938,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2893,7 +2946,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -2901,7 +2954,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -2909,7 +2962,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2917,7 +2970,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -2925,7 +2978,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2933,7 +2986,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2941,7 +2994,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2949,7 +3002,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2957,7 +3010,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2965,7 +3018,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2973,7 +3026,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2981,7 +3034,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2989,7 +3042,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2997,7 +3050,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3005,7 +3058,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3013,7 +3066,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3021,7 +3074,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3029,7 +3082,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3037,7 +3090,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3045,7 +3098,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3053,7 +3106,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -3061,7 +3114,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3069,7 +3122,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3077,7 +3130,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3085,7 +3138,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3093,7 +3146,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3101,7 +3154,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3109,7 +3162,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3117,7 +3170,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3125,7 +3178,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3133,7 +3186,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -3141,7 +3194,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3149,7 +3202,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3157,7 +3210,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -3165,7 +3218,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -3173,7 +3226,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -3181,7 +3234,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3189,7 +3242,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -3197,7 +3250,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3205,7 +3258,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3213,7 +3266,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3221,7 +3274,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3229,7 +3282,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -3237,7 +3290,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -3245,7 +3298,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3253,7 +3306,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -3261,7 +3314,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3269,7 +3322,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3277,7 +3330,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3285,7 +3338,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3293,7 +3346,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3301,7 +3354,7 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3309,7 +3362,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3317,7 +3370,7 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>

</xml_diff>

<commit_message>
Logboek bijgewerkt sheet Ruud Haertlein + Procesverslag afgemaakt
</commit_message>
<xml_diff>
--- a/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
+++ b/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ruud\Gedeelde bestanden\P4P-chatbot\Logboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ruud\Gedeelde bestanden\P4P NHL-Helpdeskbot\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>Datum</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Dictaat en planningschema doorgelezen + Start gemaakt met het functioneel ontwerp + Aanvraag verzetten deadline 6 mei FO + e-mail opdrachtgever vragen naar randvoorwaarden en overige eisen en wensen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procesverslag geschreven </t>
   </si>
 </sst>
 </file>
@@ -2762,7 +2765,7 @@
   <dimension ref="A5:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2890,11 +2893,21 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="14">
+        <v>42115</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Logboek aangepast en beveiligd logboek voor schweizer gemaakt
</commit_message>
<xml_diff>
--- a/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
+++ b/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Wander" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -141,6 +141,39 @@
   </si>
   <si>
     <t xml:space="preserve">Procesverslag geschreven </t>
+  </si>
+  <si>
+    <t>4/13/2016</t>
+  </si>
+  <si>
+    <t>4/18/2016</t>
+  </si>
+  <si>
+    <t>Opdracht meebenken en aanvullen met het opzetten van waarmee we gaan werken.</t>
+  </si>
+  <si>
+    <t>Heb de plek en tijd besproken om dit te doen</t>
+  </si>
+  <si>
+    <t>4/19/2016</t>
+  </si>
+  <si>
+    <t>Tutor en opdrachtgever gesprekken gehad, meningen gegeven over de opdracht. Daarna begonnen aan het developpen van de bot, mede door mijn groepsleden de taal bekend te maken</t>
+  </si>
+  <si>
+    <t>Kwam beetje te laat (5 min) wegens bus tijden.</t>
+  </si>
+  <si>
+    <t>4/20/2016</t>
+  </si>
+  <si>
+    <t>Grote progressie gemaakt met de bot, taakverdeling opgeschoven van het programmeren.  Commands veranderd zodat de bot reageerd op wat er gezegd wordt</t>
+  </si>
+  <si>
+    <t>Meeste van het werk wordt samen met een willekeurig andere stundend gedaan, omdat ik het meeste ervaring heb doe ik begeleiden werk, zodat iedereen even programmeerd</t>
+  </si>
+  <si>
+    <t>4/21/2016</t>
   </si>
 </sst>
 </file>
@@ -926,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,7 +993,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -980,43 +1013,97 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5">
+        <v>16</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
@@ -2764,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Logboek bijgewerkt sheet reinder
</commit_message>
<xml_diff>
--- a/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
+++ b/Logboek/Logboek - P4P - NHL-Helpdeskbot .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19296" windowHeight="7896" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wander" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>Datum</t>
   </si>
@@ -174,6 +174,24 @@
   </si>
   <si>
     <t>4/21/2016</t>
+  </si>
+  <si>
+    <t>Uitzieken</t>
+  </si>
+  <si>
+    <t>Ziek</t>
+  </si>
+  <si>
+    <t>Python code aangepast, zodat hij strings leest en onderdelen pakt en daar op antwoord.</t>
+  </si>
+  <si>
+    <t>Woensdag ochtend geen auto beschikbaar.</t>
+  </si>
+  <si>
+    <t>Zelftest gemaakt en logboek bijgewerkt.</t>
+  </si>
+  <si>
+    <t>Huiswerkdag.</t>
   </si>
 </sst>
 </file>
@@ -309,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -349,6 +367,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -959,7 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1615,7 +1639,7 @@
   <dimension ref="A5:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1627,7 +1651,7 @@
     <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1646,9 +1670,9 @@
       <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -1668,45 +1692,101 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>42473</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>42478</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>42479</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>42114</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
+        <v>42115</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5">
+        <v>16</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -2214,7 +2294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>